<commit_message>
Removed unnecessary resistors from component list
</commit_message>
<xml_diff>
--- a/src/Anchor/PCB/Onderdelenlijst.xlsx
+++ b/src/Anchor/PCB/Onderdelenlijst.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="131">
   <si>
     <t>Onderdeel</t>
   </si>
@@ -417,6 +417,9 @@
   </si>
   <si>
     <t>R LED DWM-RX</t>
+  </si>
+  <si>
+    <t>Weggelaten</t>
   </si>
 </sst>
 </file>
@@ -452,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -460,31 +463,18 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -512,66 +502,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -880,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1634,7 +1564,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>71</v>
       </c>
@@ -1657,7 +1587,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>72</v>
       </c>
@@ -1680,7 +1610,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>73</v>
       </c>
@@ -1703,7 +1633,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>74</v>
       </c>
@@ -1726,7 +1656,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -1749,7 +1679,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -1772,76 +1702,49 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="1">
-        <v>330</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D39" t="s">
-        <v>56</v>
-      </c>
-      <c r="E39" t="s">
-        <v>33</v>
-      </c>
-      <c r="F39" t="s">
-        <v>45</v>
-      </c>
-      <c r="G39" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="B39" s="4"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="1">
-        <v>330</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D40" t="s">
-        <v>56</v>
-      </c>
-      <c r="E40" t="s">
-        <v>33</v>
-      </c>
-      <c r="F40" t="s">
-        <v>45</v>
-      </c>
-      <c r="G40" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="B40" s="4"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="1">
-        <v>330</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D41" t="s">
-        <v>56</v>
-      </c>
-      <c r="E41" t="s">
-        <v>33</v>
-      </c>
-      <c r="F41" t="s">
-        <v>45</v>
-      </c>
-      <c r="G41" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B41" s="4"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -1864,7 +1767,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>81</v>
       </c>
@@ -1887,7 +1790,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>82</v>
       </c>
@@ -1910,7 +1813,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>83</v>
       </c>
@@ -1933,7 +1836,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>125</v>
       </c>
@@ -1956,7 +1859,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>126</v>
       </c>
@@ -1979,7 +1882,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>99</v>
       </c>
@@ -2188,29 +2091,30 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576 E36:E47">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"JA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>"NEE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G24:G27 F1:F1048576">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"SCHOOL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"EIGEN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48:E1048576 E1:E35">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"JA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"NEE"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Partlist changed + added seperate Anchor sketches
</commit_message>
<xml_diff>
--- a/src/Anchor/PCB/Onderdelenlijst.xlsx
+++ b/src/Anchor/PCB/Onderdelenlijst.xlsx
@@ -810,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1939,7 +1939,7 @@
         <v>106</v>
       </c>
       <c r="D50" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="E50" t="s">
         <v>33</v>

</xml_diff>